<commit_message>
test for case from freja
</commit_message>
<xml_diff>
--- a/resources/dummy_data.xlsx
+++ b/resources/dummy_data.xlsx
@@ -166,7 +166,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -378,7 +378,7 @@
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L3" activeCellId="0" sqref="L3"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -495,7 +495,7 @@
         <v>33</v>
       </c>
       <c r="L2" s="7" t="n">
-        <v>43185</v>
+        <v>7942</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>34</v>

</xml_diff>